<commit_message>
Ajustement de la note du sprint 1
</commit_message>
<xml_diff>
--- a/Equipe101.xlsx
+++ b/Equipe101.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghalichraibi/code/101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1222" documentId="13_ncr:1_{89A5CB98-93EB-451E-A012-FBFD01AD492F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6034C7B9-1748-467D-A1B6-6FB21C6586A9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F68203-E966-E34C-A5DF-7EF92C7353C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2440" yWindow="-21100" windowWidth="19200" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="146">
   <si>
     <t>Fonct.</t>
   </si>
@@ -278,10 +278,6 @@
 L'expression booléenne utilise un ou des prédicats pour simplifier une condition complexe.</t>
   </si>
   <si>
-    <t xml:space="preserve">isValidKey dans validateKeyPress aurait pu être séparé en deux prédicats (isNumberKey &amp;&amp; isNavigationKey) ou simplifié avec une liste et un include.
-</t>
-  </si>
-  <si>
     <t>7. Qualité générale</t>
   </si>
   <si>
@@ -524,7 +520,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -536,6 +532,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -573,6 +570,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -580,6 +578,7 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -587,6 +586,7 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -629,24 +629,28 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="25">
@@ -2105,6 +2109,102 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2129,104 +2229,8 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2656,17 +2660,17 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="40"/>
       <c r="B3" s="126" t="s">
         <v>0</v>
@@ -2687,7 +2691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="107" t="s">
         <v>6</v>
       </c>
@@ -2697,11 +2701,11 @@
       </c>
       <c r="C4" s="108">
         <f>'Assurance Qualité'!C59</f>
-        <v>0.76800000000000002</v>
+        <v>0.77100000000000013</v>
       </c>
       <c r="D4" s="108">
         <f>B4*0.6+C4*0.4 - 0.1*E4</f>
-        <v>0.86399999999999999</v>
+        <v>0.86519999999999997</v>
       </c>
       <c r="E4" s="109"/>
       <c r="F4" s="110">
@@ -2709,10 +2713,10 @@
       </c>
       <c r="G4" s="111">
         <f>D4*F4</f>
-        <v>17.28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>17.303999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="112" t="s">
         <v>7</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
         <v>8</v>
       </c>
@@ -2762,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="122" t="s">
         <v>9</v>
       </c>
@@ -2790,60 +2794,60 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77.5703125" style="10" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" style="10" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="10" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="10" customWidth="1"/>
-    <col min="12" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="1029" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.5" style="10" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" style="10" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="10" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="1029" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="219" t="s">
+    <row r="2" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="251" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
-      <c r="I2" s="219"/>
-      <c r="J2" s="219"/>
-      <c r="K2" s="219"/>
+      <c r="B2" s="251"/>
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="251"/>
+      <c r="J2" s="251"/>
+      <c r="K2" s="251"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="220" t="s">
+    <row r="4" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="252" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="220"/>
-      <c r="C4" s="220"/>
-      <c r="D4" s="220"/>
-      <c r="E4" s="220"/>
-      <c r="F4" s="220"/>
-      <c r="G4" s="220"/>
-      <c r="H4" s="220"/>
-      <c r="I4" s="220"/>
-      <c r="J4" s="220"/>
-      <c r="K4" s="220"/>
+      <c r="B4" s="252"/>
+      <c r="C4" s="252"/>
+      <c r="D4" s="252"/>
+      <c r="E4" s="252"/>
+      <c r="F4" s="252"/>
+      <c r="G4" s="252"/>
+      <c r="H4" s="252"/>
+      <c r="I4" s="252"/>
+      <c r="J4" s="252"/>
+      <c r="K4" s="252"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="18.75">
+    <row r="5" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="41"/>
       <c r="C5" s="2"/>
@@ -2858,37 +2862,37 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="237" t="s">
+    <row r="6" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="244" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="224" t="s">
+      <c r="B6" s="256" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="239" t="s">
+      <c r="C6" s="246" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="240"/>
-      <c r="E6" s="240"/>
-      <c r="F6" s="241" t="s">
+      <c r="D6" s="247"/>
+      <c r="E6" s="247"/>
+      <c r="F6" s="248" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="242"/>
-      <c r="H6" s="243"/>
-      <c r="I6" s="221" t="s">
+      <c r="G6" s="249"/>
+      <c r="H6" s="250"/>
+      <c r="I6" s="253" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="222"/>
-      <c r="K6" s="223"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="255"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="236"/>
-      <c r="P6" s="236"/>
-    </row>
-    <row r="7" spans="1:17" ht="18.75">
-      <c r="A7" s="238"/>
-      <c r="B7" s="225"/>
+      <c r="N6" s="242"/>
+      <c r="O6" s="243"/>
+      <c r="P6" s="243"/>
+    </row>
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="245"/>
+      <c r="B7" s="257"/>
       <c r="C7" s="14" t="s">
         <v>14</v>
       </c>
@@ -2923,27 +2927,27 @@
       <c r="P7" s="40"/>
       <c r="Q7" s="40"/>
     </row>
-    <row r="8" spans="1:17" ht="18.75">
-      <c r="A8" s="234" t="s">
+    <row r="8" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="226" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="234"/>
-      <c r="C8" s="227" t="s">
+      <c r="B8" s="226"/>
+      <c r="C8" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="228"/>
+      <c r="D8" s="220"/>
       <c r="E8" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="227" t="s">
+      <c r="F8" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="228"/>
+      <c r="G8" s="220"/>
       <c r="H8" s="46"/>
-      <c r="I8" s="227" t="s">
+      <c r="I8" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="228"/>
+      <c r="J8" s="220"/>
       <c r="K8" s="46"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -2952,7 +2956,7 @@
       <c r="P8" s="40"/>
       <c r="Q8" s="40"/>
     </row>
-    <row r="9" spans="1:17" ht="45.75">
+    <row r="9" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>19</v>
       </c>
@@ -2983,7 +2987,7 @@
       <c r="P9" s="40"/>
       <c r="Q9" s="40"/>
     </row>
-    <row r="10" spans="1:17" ht="30.75">
+    <row r="10" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>21</v>
       </c>
@@ -3014,11 +3018,11 @@
       <c r="P10" s="40"/>
       <c r="Q10" s="40"/>
     </row>
-    <row r="11" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A11" s="229" t="s">
+    <row r="11" spans="1:17" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="230"/>
+      <c r="B11" s="222"/>
       <c r="C11" s="47">
         <f>SUMPRODUCT(C6:C10,D6:D10)</f>
         <v>8</v>
@@ -3053,27 +3057,27 @@
       <c r="P11" s="44"/>
       <c r="Q11" s="44"/>
     </row>
-    <row r="12" spans="1:17" s="12" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="234" t="s">
+    <row r="12" spans="1:17" s="12" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="226" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="234"/>
-      <c r="C12" s="227" t="s">
+      <c r="B12" s="226"/>
+      <c r="C12" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="228"/>
+      <c r="D12" s="220"/>
       <c r="E12" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="227" t="s">
+      <c r="F12" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="228"/>
+      <c r="G12" s="220"/>
       <c r="H12" s="46"/>
-      <c r="I12" s="227" t="s">
+      <c r="I12" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="228"/>
+      <c r="J12" s="220"/>
       <c r="K12" s="46"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3082,7 +3086,7 @@
       <c r="P12" s="43"/>
       <c r="Q12" s="43"/>
     </row>
-    <row r="13" spans="1:17" ht="60.75">
+    <row r="13" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>26</v>
       </c>
@@ -3113,7 +3117,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="76.5">
+    <row r="14" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>29</v>
       </c>
@@ -3144,7 +3148,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="198">
+    <row r="15" spans="1:17" ht="192" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>32</v>
       </c>
@@ -3175,7 +3179,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="30.75">
+    <row r="16" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>35</v>
       </c>
@@ -3204,7 +3208,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="121.5">
+    <row r="17" spans="1:17" ht="128" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>37</v>
       </c>
@@ -3235,11 +3239,11 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A18" s="229" t="s">
+    <row r="18" spans="1:17" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="230"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="47">
         <f>SUMPRODUCT(C13:C17,D13:D17)</f>
         <v>8.9499999999999993</v>
@@ -3274,32 +3278,32 @@
       <c r="P18" s="44"/>
       <c r="Q18" s="44"/>
     </row>
-    <row r="19" spans="1:17" s="43" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A19" s="226" t="s">
+    <row r="19" spans="1:17" s="43" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="258" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="226"/>
-      <c r="C19" s="227" t="s">
+      <c r="B19" s="258"/>
+      <c r="C19" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="228"/>
+      <c r="D19" s="220"/>
       <c r="E19" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="227" t="s">
+      <c r="F19" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="228"/>
+      <c r="G19" s="220"/>
       <c r="H19" s="46"/>
-      <c r="I19" s="227" t="s">
+      <c r="I19" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="228"/>
+      <c r="J19" s="220"/>
       <c r="K19" s="46"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:17" ht="229.5">
+    <row r="20" spans="1:17" ht="128" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>42</v>
       </c>
@@ -3328,7 +3332,7 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:17" ht="30.75">
+    <row r="21" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>45</v>
       </c>
@@ -3355,11 +3359,11 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A22" s="231" t="s">
+    <row r="22" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="232"/>
+      <c r="B22" s="241"/>
       <c r="C22" s="57">
         <f>SUMPRODUCT(C20:C21,D20:D21)</f>
         <v>3</v>
@@ -3390,32 +3394,32 @@
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
     </row>
-    <row r="23" spans="1:17" ht="18.75" customHeight="1">
+    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="214" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="214"/>
-      <c r="C23" s="227" t="s">
+      <c r="C23" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="228"/>
+      <c r="D23" s="220"/>
       <c r="E23" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="227" t="s">
+      <c r="F23" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="228"/>
+      <c r="G23" s="220"/>
       <c r="H23" s="46"/>
-      <c r="I23" s="227" t="s">
+      <c r="I23" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="228"/>
+      <c r="J23" s="220"/>
       <c r="K23" s="46"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:17" ht="30.75">
+    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="42" t="s">
         <v>48</v>
       </c>
@@ -3442,7 +3446,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
         <v>50</v>
       </c>
@@ -3471,7 +3475,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>53</v>
       </c>
@@ -3498,11 +3502,11 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A27" s="233" t="s">
+    <row r="27" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="240" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="232"/>
+      <c r="B27" s="241"/>
       <c r="C27" s="47">
         <f>SUMPRODUCT(C24:C26,D24:D26)</f>
         <v>3.8</v>
@@ -3533,32 +3537,32 @@
       <c r="L27" s="56"/>
       <c r="M27" s="56"/>
     </row>
-    <row r="28" spans="1:17" ht="21" customHeight="1">
-      <c r="A28" s="226" t="s">
+    <row r="28" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="258" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="226"/>
-      <c r="C28" s="227">
+      <c r="B28" s="258"/>
+      <c r="C28" s="219">
         <v>1</v>
       </c>
-      <c r="D28" s="228"/>
+      <c r="D28" s="220"/>
       <c r="E28" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="227" t="s">
+      <c r="F28" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="228"/>
+      <c r="G28" s="220"/>
       <c r="H28" s="66"/>
-      <c r="I28" s="227" t="s">
+      <c r="I28" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="228"/>
+      <c r="J28" s="220"/>
       <c r="K28" s="46"/>
       <c r="L28" s="9"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:17" ht="91.5">
+    <row r="29" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
@@ -3589,7 +3593,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
         <v>59</v>
       </c>
@@ -3618,7 +3622,7 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:17" ht="30.75">
+    <row r="31" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>61</v>
       </c>
@@ -3647,11 +3651,11 @@
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
     </row>
-    <row r="32" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A32" s="229" t="s">
+    <row r="32" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="230"/>
+      <c r="B32" s="222"/>
       <c r="C32" s="47">
         <f>SUMPRODUCT(C29:C31,D29:D31)</f>
         <v>5.4</v>
@@ -3682,22 +3686,22 @@
       <c r="L32" s="56"/>
       <c r="M32" s="56"/>
     </row>
-    <row r="33" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A33" s="234" t="s">
+    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="226" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="234"/>
-      <c r="C33" s="227" t="s">
+      <c r="B33" s="226"/>
+      <c r="C33" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="228"/>
+      <c r="D33" s="220"/>
       <c r="E33" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="227" t="s">
+      <c r="F33" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="228"/>
+      <c r="G33" s="220"/>
       <c r="H33" s="46"/>
       <c r="I33" s="68" t="s">
         <v>17</v>
@@ -3707,7 +3711,7 @@
       <c r="L33" s="8"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="1:13" ht="30.75">
+    <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="s">
         <v>64</v>
       </c>
@@ -3734,7 +3738,7 @@
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>66</v>
       </c>
@@ -3761,7 +3765,7 @@
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
         <v>68</v>
       </c>
@@ -3790,7 +3794,7 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="1:13" ht="91.5">
+    <row r="37" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
         <v>71</v>
       </c>
@@ -3798,14 +3802,12 @@
         <v>72</v>
       </c>
       <c r="C37" s="83">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D37" s="84">
         <v>3</v>
       </c>
-      <c r="E37" s="85" t="s">
-        <v>73</v>
-      </c>
+      <c r="E37" s="85"/>
       <c r="F37" s="86"/>
       <c r="G37" s="87">
         <v>3</v>
@@ -3819,14 +3821,14 @@
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" s="44" customFormat="1" ht="15.75">
-      <c r="A38" s="229" t="s">
+    <row r="38" spans="1:13" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="230"/>
+      <c r="B38" s="222"/>
       <c r="C38" s="69">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
-        <v>9.25</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="D38" s="48">
         <f>SUM(D34:D37)</f>
@@ -3854,37 +3856,37 @@
       <c r="L38" s="56"/>
       <c r="M38" s="56"/>
     </row>
-    <row r="39" spans="1:13" ht="18.75" customHeight="1">
+    <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="45"/>
+      <c r="C39" s="219" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="220"/>
+      <c r="E39" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="227" t="s">
+      <c r="F39" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="228"/>
-      <c r="E39" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="227" t="s">
+      <c r="G39" s="220"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="228"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="227" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="228"/>
+      <c r="J39" s="220"/>
       <c r="K39" s="46"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" ht="60.75">
+    <row r="40" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="23" t="s">
         <v>76</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>77</v>
       </c>
       <c r="C40" s="83">
         <v>1</v>
@@ -3910,12 +3912,12 @@
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
     </row>
-    <row r="41" spans="1:13" ht="91.5">
+    <row r="41" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>78</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>79</v>
       </c>
       <c r="C41" s="83">
         <v>0.7</v>
@@ -3924,7 +3926,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F41" s="86"/>
       <c r="G41" s="87">
@@ -3941,12 +3943,12 @@
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="23" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>82</v>
       </c>
       <c r="C42" s="83">
         <v>1</v>
@@ -3971,12 +3973,12 @@
       <c r="K42" s="78"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:13" ht="60.75">
+    <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="23" t="s">
         <v>83</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>84</v>
       </c>
       <c r="C43" s="83">
         <v>0.8</v>
@@ -3985,7 +3987,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F43" s="86"/>
       <c r="G43" s="87">
@@ -4002,12 +4004,12 @@
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
     </row>
-    <row r="44" spans="1:13" ht="167.25">
+    <row r="44" spans="1:13" ht="128" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="23" t="s">
         <v>86</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>87</v>
       </c>
       <c r="C44" s="83">
         <v>0</v>
@@ -4016,7 +4018,7 @@
         <v>6</v>
       </c>
       <c r="E44" s="85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F44" s="86"/>
       <c r="G44" s="87">
@@ -4033,12 +4035,12 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="45.75">
+    <row r="45" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="23" t="s">
         <v>89</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>90</v>
       </c>
       <c r="C45" s="83">
         <v>1</v>
@@ -4064,12 +4066,12 @@
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
     </row>
-    <row r="46" spans="1:13" ht="30.75">
+    <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="23" t="s">
         <v>91</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>92</v>
       </c>
       <c r="C46" s="83">
         <v>1</v>
@@ -4095,12 +4097,12 @@
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
     </row>
-    <row r="47" spans="1:13" ht="321">
+    <row r="47" spans="1:13" ht="192" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="23" t="s">
         <v>93</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>94</v>
       </c>
       <c r="C47" s="83">
         <v>0.3</v>
@@ -4109,7 +4111,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F47" s="86"/>
       <c r="G47" s="87">
@@ -4126,12 +4128,12 @@
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="23" t="s">
         <v>96</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>97</v>
       </c>
       <c r="C48" s="83">
         <v>1</v>
@@ -4157,11 +4159,11 @@
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
     </row>
-    <row r="49" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A49" s="229" t="s">
+    <row r="49" spans="1:17" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="230"/>
+      <c r="B49" s="222"/>
       <c r="C49" s="71">
         <f>SUMPRODUCT(C40:C48,D40:D48)</f>
         <v>28.400000000000002</v>
@@ -4196,37 +4198,37 @@
       <c r="P49" s="44"/>
       <c r="Q49" s="44"/>
     </row>
-    <row r="50" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A50" s="234" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="234"/>
-      <c r="C50" s="227" t="s">
+    <row r="50" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="226" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="226"/>
+      <c r="C50" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="228"/>
+      <c r="D50" s="220"/>
       <c r="E50" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="F50" s="227" t="s">
+      <c r="F50" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="228"/>
+      <c r="G50" s="220"/>
       <c r="H50" s="46"/>
-      <c r="I50" s="227" t="s">
+      <c r="I50" s="219" t="s">
         <v>17</v>
       </c>
-      <c r="J50" s="228"/>
+      <c r="J50" s="220"/>
       <c r="K50" s="46"/>
       <c r="L50" s="8"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>100</v>
       </c>
       <c r="C51" s="79">
         <v>1</v>
@@ -4248,12 +4250,12 @@
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="23" t="s">
         <v>101</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>102</v>
       </c>
       <c r="C52" s="83">
         <v>1</v>
@@ -4275,12 +4277,12 @@
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
     </row>
-    <row r="53" spans="1:17" ht="30.75">
+    <row r="53" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="23" t="s">
         <v>103</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>104</v>
       </c>
       <c r="C53" s="83">
         <v>1</v>
@@ -4302,12 +4304,12 @@
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
     </row>
-    <row r="54" spans="1:17" ht="60.75">
+    <row r="54" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="23" t="s">
         <v>105</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>106</v>
       </c>
       <c r="C54" s="83">
         <v>1</v>
@@ -4329,12 +4331,12 @@
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
     </row>
-    <row r="55" spans="1:17" ht="45.75">
+    <row r="55" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="23" t="s">
         <v>107</v>
-      </c>
-      <c r="B55" s="23" t="s">
-        <v>108</v>
       </c>
       <c r="C55" s="83">
         <v>0.5</v>
@@ -4343,7 +4345,7 @@
         <v>2</v>
       </c>
       <c r="E55" s="85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F55" s="86"/>
       <c r="G55" s="87">
@@ -4358,11 +4360,11 @@
       <c r="L55" s="6"/>
       <c r="M55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A56" s="229" t="s">
+    <row r="56" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="B56" s="230"/>
+      <c r="B56" s="222"/>
       <c r="C56" s="57">
         <f>SUMPRODUCT(C51:C55,D51:D55)</f>
         <v>10</v>
@@ -4393,31 +4395,31 @@
       <c r="L56" s="56"/>
       <c r="M56" s="56"/>
     </row>
-    <row r="57" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A57" s="257" t="s">
+    <row r="57" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="258"/>
-      <c r="C57" s="258"/>
-      <c r="D57" s="258"/>
-      <c r="E57" s="258"/>
-      <c r="F57" s="258"/>
-      <c r="G57" s="258"/>
-      <c r="H57" s="258"/>
-      <c r="I57" s="258"/>
-      <c r="J57" s="258"/>
-      <c r="K57" s="259"/>
+      <c r="B57" s="224"/>
+      <c r="C57" s="224"/>
+      <c r="D57" s="224"/>
+      <c r="E57" s="224"/>
+      <c r="F57" s="224"/>
+      <c r="G57" s="224"/>
+      <c r="H57" s="224"/>
+      <c r="I57" s="224"/>
+      <c r="J57" s="224"/>
+      <c r="K57" s="225"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:17">
-      <c r="A58" s="244" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="245"/>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="227" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="228"/>
       <c r="C58" s="34">
         <f>C11+C18+C22+C27+C32+C38+C49+C56</f>
-        <v>76.8</v>
+        <v>77.100000000000009</v>
       </c>
       <c r="D58" s="25">
         <f>D11+D18+D22+D27+D32+D38+D49+D56</f>
@@ -4445,53 +4447,50 @@
       <c r="L58" s="6"/>
       <c r="M58" s="5"/>
     </row>
-    <row r="59" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A59" s="246" t="s">
-        <v>111</v>
-      </c>
-      <c r="B59" s="247"/>
-      <c r="C59" s="248">
+    <row r="59" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="229" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="230"/>
+      <c r="C59" s="231">
         <f>C58/D58</f>
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="D59" s="249"/>
-      <c r="E59" s="250"/>
-      <c r="F59" s="251">
+        <v>0.77100000000000013</v>
+      </c>
+      <c r="D59" s="232"/>
+      <c r="E59" s="233"/>
+      <c r="F59" s="234">
         <f>F58/G58</f>
         <v>0</v>
       </c>
-      <c r="G59" s="252"/>
-      <c r="H59" s="253"/>
-      <c r="I59" s="254">
+      <c r="G59" s="235"/>
+      <c r="H59" s="236"/>
+      <c r="I59" s="237">
         <f>I58/J58</f>
         <v>0</v>
       </c>
-      <c r="J59" s="255"/>
-      <c r="K59" s="256"/>
+      <c r="J59" s="238"/>
+      <c r="K59" s="239"/>
       <c r="L59" s="72"/>
       <c r="M59" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="N6:P6"/>
@@ -4508,22 +4507,25 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L18 L22 L27 L32 L38 L49 L11 C9:C10 F9:F10 I9:I10 C24:C26 F24:F26 I24:I26 C34:C37 F34:F37 I34:I37 C51:C55 F51:F55 I51:I55 I13:I17 F13:F17 C13:C17 I20:I21 F20:F21 C20:C21 I29:I31 F29:F31 C29:C31 I40:I48 F40:F48 C40:C48" xr:uid="{4A0D4DC8-F6F9-4765-AB49-E4E0ACDB1361}">
@@ -4549,18 +4551,18 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" style="37" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="37"/>
-    <col min="4" max="4" width="9.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5" style="37" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" style="37"/>
+    <col min="4" max="4" width="9.83203125" style="37" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="37" customWidth="1"/>
-    <col min="7" max="7" width="54.85546875" style="37" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="37"/>
+    <col min="7" max="7" width="54.83203125" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="37"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="18.75">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="260" t="s">
         <v>10</v>
       </c>
@@ -4571,7 +4573,7 @@
       <c r="F2" s="260"/>
       <c r="G2" s="260"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="39"/>
@@ -4580,9 +4582,9 @@
       <c r="F3" s="38"/>
       <c r="G3" s="39"/>
     </row>
-    <row r="4" spans="1:7" ht="18.75">
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -4591,8 +4593,8 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="6" spans="1:7" ht="23.25">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="264" t="s">
         <v>6</v>
       </c>
@@ -4603,21 +4605,21 @@
       <c r="F6" s="265"/>
       <c r="G6" s="266"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="130" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="131" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="131" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="131" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7" s="131" t="s">
         <v>17</v>
@@ -4626,9 +4628,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="133" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="134">
         <v>1</v>
@@ -4648,9 +4650,9 @@
       </c>
       <c r="G8" s="135"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="136" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="137">
         <v>1</v>
@@ -4670,9 +4672,9 @@
       </c>
       <c r="G9" s="138"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="134">
         <v>1</v>
@@ -4692,9 +4694,9 @@
       </c>
       <c r="G10" s="135"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="136" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="137">
         <v>0.8</v>
@@ -4713,12 +4715,12 @@
         <v>18</v>
       </c>
       <c r="G11" s="138" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="133" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="133" t="s">
-        <v>121</v>
       </c>
       <c r="B12" s="134">
         <v>0.8</v>
@@ -4737,12 +4739,12 @@
         <v>18</v>
       </c>
       <c r="G12" s="135" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="133" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="133" t="s">
-        <v>123</v>
       </c>
       <c r="B13" s="134">
         <v>1</v>
@@ -4762,9 +4764,9 @@
       </c>
       <c r="G13" s="135"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="136" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="137">
         <v>1</v>
@@ -4784,9 +4786,9 @@
       </c>
       <c r="G14" s="138"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="139" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B15" s="267"/>
       <c r="C15" s="267"/>
@@ -4801,9 +4803,9 @@
       <c r="F15" s="141"/>
       <c r="G15" s="142"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="143" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="144" t="s">
         <v>14</v>
@@ -4813,16 +4815,16 @@
         <v>4</v>
       </c>
       <c r="E16" s="145" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16" s="145"/>
       <c r="G16" s="146" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="147" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="148"/>
       <c r="C17" s="148"/>
@@ -4838,9 +4840,9 @@
       </c>
       <c r="G17" s="150"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="151" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="152">
         <v>0</v>
@@ -4856,7 +4858,7 @@
       <c r="F18" s="152"/>
       <c r="G18" s="154"/>
     </row>
-    <row r="19" spans="1:7" ht="23.25">
+    <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="268" t="s">
         <v>7</v>
       </c>
@@ -4867,21 +4869,21 @@
       <c r="F19" s="269"/>
       <c r="G19" s="270"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="156" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="156" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" s="156" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="156" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F20" s="156" t="s">
         <v>17</v>
@@ -4890,9 +4892,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="158" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="159">
         <v>0</v>
@@ -4910,9 +4912,9 @@
       <c r="F21" s="159"/>
       <c r="G21" s="160"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="161" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B22" s="162">
         <v>0</v>
@@ -4924,15 +4926,15 @@
         <v>14</v>
       </c>
       <c r="E22" s="162">
-        <f t="shared" ref="E22:E28" si="1">B22*C22*D22</f>
+        <f t="shared" ref="E22:E27" si="1">B22*C22*D22</f>
         <v>0</v>
       </c>
       <c r="F22" s="162"/>
       <c r="G22" s="163"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="158" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="159">
         <v>0</v>
@@ -4950,9 +4952,9 @@
       <c r="F23" s="159"/>
       <c r="G23" s="160"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="161" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="162">
         <v>0</v>
@@ -4970,9 +4972,9 @@
       <c r="F24" s="162"/>
       <c r="G24" s="163"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="158" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="159">
         <v>0</v>
@@ -4990,9 +4992,9 @@
       <c r="F25" s="159"/>
       <c r="G25" s="160"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="161" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="162">
         <v>0</v>
@@ -5010,9 +5012,9 @@
       <c r="F26" s="162"/>
       <c r="G26" s="163"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="215" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="215">
         <v>0</v>
@@ -5030,9 +5032,9 @@
       <c r="F27" s="215"/>
       <c r="G27" s="216"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="164" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B28" s="165"/>
       <c r="C28" s="165"/>
@@ -5047,9 +5049,9 @@
       <c r="F28" s="166"/>
       <c r="G28" s="167"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="168" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B29" s="169" t="s">
         <v>14</v>
@@ -5059,16 +5061,16 @@
         <v>4</v>
       </c>
       <c r="E29" s="170" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F29" s="170"/>
       <c r="G29" s="171" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="172" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="173">
         <v>0</v>
@@ -5084,9 +5086,9 @@
       <c r="F30" s="173"/>
       <c r="G30" s="175"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="176" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="177">
         <v>0</v>
@@ -5102,9 +5104,9 @@
       <c r="F31" s="177"/>
       <c r="G31" s="179"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="180" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" s="181">
         <v>0</v>
@@ -5120,7 +5122,7 @@
       <c r="F32" s="181"/>
       <c r="G32" s="183"/>
     </row>
-    <row r="33" spans="1:7" ht="23.25">
+    <row r="33" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A33" s="261" t="s">
         <v>8</v>
       </c>
@@ -5131,21 +5133,21 @@
       <c r="F33" s="262"/>
       <c r="G33" s="263"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="184" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="185" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="185" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" s="185" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="185" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F34" s="185" t="s">
         <v>17</v>
@@ -5154,9 +5156,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="187" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" s="188">
         <v>0</v>
@@ -5174,9 +5176,9 @@
       <c r="F35" s="188"/>
       <c r="G35" s="189"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="190" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" s="191">
         <v>0</v>
@@ -5194,9 +5196,9 @@
       <c r="F36" s="191"/>
       <c r="G36" s="192"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="187" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" s="188">
         <v>0</v>
@@ -5214,9 +5216,9 @@
       <c r="F37" s="188"/>
       <c r="G37" s="189"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="190" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B38" s="191">
         <v>0</v>
@@ -5234,9 +5236,9 @@
       <c r="F38" s="191"/>
       <c r="G38" s="192"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="187" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39" s="188">
         <v>0</v>
@@ -5254,9 +5256,9 @@
       <c r="F39" s="188"/>
       <c r="G39" s="189"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="190" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="191">
         <v>0</v>
@@ -5274,9 +5276,9 @@
       <c r="F40" s="191"/>
       <c r="G40" s="192"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="187" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B41" s="188">
         <v>0</v>
@@ -5294,9 +5296,9 @@
       <c r="F41" s="188"/>
       <c r="G41" s="189"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="217" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B42" s="217">
         <v>0</v>
@@ -5314,9 +5316,9 @@
       <c r="F42" s="217"/>
       <c r="G42" s="217"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="193" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" s="194"/>
       <c r="C43" s="194"/>
@@ -5331,9 +5333,9 @@
       <c r="F43" s="195"/>
       <c r="G43" s="196"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="197" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" s="198" t="s">
         <v>14</v>
@@ -5343,16 +5345,16 @@
         <v>4</v>
       </c>
       <c r="E44" s="199" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F44" s="199"/>
       <c r="G44" s="200" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="201" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B45" s="202">
         <v>0</v>
@@ -5368,9 +5370,9 @@
       <c r="F45" s="202"/>
       <c r="G45" s="204"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="205" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B46" s="206">
         <v>0</v>
@@ -5386,9 +5388,9 @@
       <c r="F46" s="206"/>
       <c r="G46" s="208"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="209" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="210">
         <v>0</v>
@@ -5431,6 +5433,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B41E0342602C49449CD93109DBCAB8C5" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cab946e3812a26735e8b0dc00d59aca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3ea4e87-b30d-4ccc-9564-7710f23c54f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afa808ced5dc9827eedaaa69eb8b35dd" ns2:_="">
     <xsd:import namespace="d3ea4e87-b30d-4ccc-9564-7710f23c54f0"/>
@@ -5562,29 +5579,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3ea4e87-b30d-4ccc-9564-7710f23c54f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore: added updated scores sprint2
</commit_message>
<xml_diff>
--- a/Equipe101.xlsx
+++ b/Equipe101.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghalichraibi/code/101/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamel/Documents/SchoolWork/Charge2990/LOG2990-101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F68203-E966-E34C-A5DF-7EF92C7353C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B864263C-1558-2441-A221-2AC54E202997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2440" yWindow="-21100" windowWidth="19200" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
     <sheet name="Assurance Qualité" sheetId="6" r:id="rId2"/>
     <sheet name="Fonctionnalités" sheetId="8" r:id="rId3"/>
+    <sheet name="Documents" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="191">
   <si>
     <t>Fonct.</t>
   </si>
@@ -59,6 +60,9 @@
     <t>Note pondérée</t>
   </si>
   <si>
+    <t>Documents</t>
+  </si>
+  <si>
     <t>Sprint 1</t>
   </si>
   <si>
@@ -102,6 +106,9 @@
   </si>
   <si>
     <t>Le projet respecte les meilleures pratiques des cadriciels utilisés. (Exemple: séparation des responsabilités dans les Components et Services d'Angular, respect de la sémantique HTTP avec Express, etc.)</t>
+  </si>
+  <si>
+    <t>Attention au Style dans le html de CanvasTopButtonsComponent</t>
   </si>
   <si>
     <t>1.2 Arborescence</t>
@@ -127,6 +134,9 @@
   </si>
   <si>
     <t>GameAreaService a beaucoup trop de responsabilité. Il serait important d'en moins extraire la logique de la musique dans un autre service.</t>
+  </si>
+  <si>
+    <t>ClassicModeService peut être fragmentée davantage en séparant ses différents rôles dans des services (timer, gestion/creation des rooms, verifications des coordonnes, gestion de la waitlist, ...)</t>
   </si>
   <si>
     <t>2.2 Attributs</t>
@@ -141,6 +151,13 @@
 config-page.component.ts: titre non utilisé</t>
   </si>
   <si>
+    <t>GamePageComponent a beaucoup d'attributs, prenez le temps de les encapsuler dans des types/classes.
+Attributs non utilisés:
+canvas-top-buttons.component.ts: operationDetails, position
+game-infos.component.ts: playerName
+canvas-middle-buttons.component.ts: canvasPosition</t>
+  </si>
+  <si>
     <t>2.3 Accessibilité</t>
   </si>
   <si>
@@ -151,6 +168,18 @@
     <t>Plusieurs méthodes de difference.service.ts devraient être private (enlargeDifferences, breadthFirstSearch, etc.)
 image.service.ts: transformImageDataToPixelsArray, transformPixel... servent à simplifier le code de votre classe, donc elles doivent être private.
 convert2DCoordToPixel doit être aussi private</t>
+  </si>
+  <si>
+    <t>Vous devez déclarer les attributs des composants comme privés s'ils ne sont pas utilisés à l'extérieur. Cela permet d'encapsuler les détails d'implémentation et de réduire la dépendance avec les autres composants.
+Voici une liste de components à modifier:
+canvas-top-buttons.component.ts: operationDetails
+chat-box.component.ts: add, oneVsOneGameMode
+nav-bar.component.ts: gameRoute
+canvas-middle-buttons.component.ts: canvasPosition
+selection-page.component.ts: selectionRoute
+main-page.component.ts: gameRoute
+config-page.component.ts: homeRoute
+Vous avez aussi plusieurs méthodes qui doivent suivre le même principe</t>
   </si>
   <si>
     <t>2.4 Couplage</t>
@@ -175,6 +204,9 @@
 etc.</t>
   </si>
   <si>
+    <t>creation-game-dialog.component.ts</t>
+  </si>
+  <si>
     <t>3. Fonctions et méthodes</t>
   </si>
   <si>
@@ -189,7 +221,13 @@
 La fonction n'a pas une longueur trop grande.</t>
   </si>
   <si>
-    <t>setImageIfValid est triviale (canvas-under-buttons), isNumberOfDifferencesValid est triviale, onNoClick est inutile si dialogRef est public (creation-game-dialog),  showDialog ne devrait pas être dans les services (services multiples), flashCorrectPixels est trop longue (game-area), etc.</t>
+    <t>setImageIfValid est triviale (canvas-under-buttons), isNumberOfDifferencesValid est triviale, onNoClick est inutile si dialogRef est public (player-name-dialog-box),  showDialog ne devrait pas être dans les services (services multiples), flashCorrectPixels est trop longue (game-area), etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canvas-top-buttons: ngAfterViewInit triviale, 
+Validation-service: isImageTypeValid et isImageFormatValid sont triviales.
+Classic-mode-service serveur: verifyCoords trop longue, peut-être fragmentée
+</t>
   </si>
   <si>
     <t>3.2 Paramètres</t>
@@ -235,6 +273,9 @@
     <t>flashCorrectPixels chiffres magiques (game-area), default best times dans la classe (game-lists-manager)</t>
   </si>
   <si>
+    <t>Bien!</t>
+  </si>
+  <si>
     <t>5.2 Environnement</t>
   </si>
   <si>
@@ -247,6 +288,9 @@
     <t>La constante est utilisé dans un contexte lié à la logique d'affaire. (Exemple d'erreur: const DEUX = 2,  bonne utilisation: WAIT_TIME = 5000 )</t>
   </si>
   <si>
+    <t>Constants.ts: ONE_SECOND, TEN_SECONDS</t>
+  </si>
+  <si>
     <t>6. Expressions booléennes</t>
   </si>
   <si>
@@ -256,6 +300,9 @@
     <t>L'expression booléenne n'es pas comparée à true ou false. (Exemple d'erreur: x === true)</t>
   </si>
   <si>
+    <t>chat-box.component.ts: 22</t>
+  </si>
+  <si>
     <t>6.2 Logique négative</t>
   </si>
   <si>
@@ -269,6 +316,9 @@
   </si>
   <si>
     <t>game-area.service.ts: 69</t>
+  </si>
+  <si>
+    <t>player-name-dialog-box.component.ts: 55</t>
   </si>
   <si>
     <t>6.4 Prédicats</t>
@@ -276,6 +326,12 @@
   <si>
     <t>L'expression booléenne est simple.
 L'expression booléenne utilise un ou des prédicats pour simplifier une condition complexe.</t>
+  </si>
+  <si>
+    <t>classic-mode.service.ts: 157</t>
+  </si>
+  <si>
+    <t>Très bon travail !</t>
   </si>
   <si>
     <t>7. Qualité générale</t>
@@ -306,6 +362,10 @@
   </si>
   <si>
     <t>Le code utilise des enum lorsque c'est pertinent.</t>
+  </si>
+  <si>
+    <t>Mike:
+Bon travail</t>
   </si>
   <si>
     <t>7.4 Classe et interface</t>
@@ -329,6 +389,12 @@
 setLeftBackground et
 setRightBackground
 getLeftPixels et getRightPixels</t>
+  </si>
+  <si>
+    <t>Mike:
+getSoloDifferenceMessage et getOneVsOneDifferenceMessage ( le message doit changer en fonction du mode, cela peut etre fait en une seule fonction)
+getSoloErrorMessage et getOneVsOneErrorMessage pareil ici
+Votre constructor et ngAfterViewInit de CanvasTopButtomComponent contient du code dupliqué</t>
   </si>
   <si>
     <t>7.6 ESLint</t>
@@ -360,6 +426,13 @@
 hasNext et hasPrevious font penser a des fonctions booléennes mais n'ont pas de type de retour booléen ( confusion)</t>
   </si>
   <si>
+    <t xml:space="preserve">Mike:
+Évitez les abréviation Og et Md et diff
+isPlayerNameTaken devrait être de type boolean
+verifyCoords fait penser qui doit retourner une valeur pour vérification
+fonction gameCardDeleted est une fonction void qui ne décrit pas une verbe d'action </t>
+  </si>
+  <si>
     <t>7.8 Performance</t>
   </si>
   <si>
@@ -405,6 +478,9 @@
 </t>
   </si>
   <si>
+    <t>Super maintien du git!</t>
+  </si>
+  <si>
     <t>Total QA sprint</t>
   </si>
   <si>
@@ -465,9 +541,16 @@
     <t>2.1 Vue de création de jeu - modification de l'avant-plan</t>
   </si>
   <si>
+    <t>problème avec le bouton shift après le dernier clic</t>
+  </si>
+  <si>
     <t>2.2 Créer et Joindre une partie un contre un</t>
   </si>
   <si>
+    <t>Le cas ou on quitte la page quand on attend un joueur n'annule pas la demande de création de jeu
+ donc l'autre ne sait pas qu'il doit plus attendre et la game est locked ( faut shutdown server)</t>
+  </si>
+  <si>
     <t>2.3 Mode Classique en un contre un</t>
   </si>
   <si>
@@ -514,13 +597,137 @@
   </si>
   <si>
     <t>Erreur de build / déploiement erroné</t>
+  </si>
+  <si>
+    <t>Document d'Architecture</t>
+  </si>
+  <si>
+    <t>Protocole de communication</t>
+  </si>
+  <si>
+    <t>Historique des révisions</t>
+  </si>
+  <si>
+    <t>Vous avez plusieurs fois la version 1.1 et 1.3</t>
+  </si>
+  <si>
+    <t>1 Introduction /1</t>
+  </si>
+  <si>
+    <t>Bien</t>
+  </si>
+  <si>
+    <t>1 Introduction (commentaires)</t>
+  </si>
+  <si>
+    <t>2 Vue des cas d'utilisation /5</t>
+  </si>
+  <si>
+    <t>2 Communication client-serveur /7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 1 : manque des relations "extends" pour CU-7.0 et CU-1.0. CU-1.0 doit être possible seulement en mode Solo
+Figure 2 : CU-1.2 trop bas niveau (à retirer). La relation entre "Jouer une partie" et CU-1.2 est un "extend" : le joueur n'est pas forcé de consulter l'historique après chaque partie. CU-2.2.X : trop bas niveau (à retirer).
+Figure 3 : CU-3.0 et CU-3.1 devrait être inversés. CU-3.2 à retirer : quelle est la différence entre "configurer" et "modifier" ? CU-4.2 est un détail d'implémentation et une séquence (à retirer).
+Figure 4 : CU-7.1.X : trop bas niveau (à retirer). CU -7.2.1 : pourquoi est-ce la seule action spécifiée (à retirer)
+Figure 8: relation "include" dans le vide à partir du CU-8.0. </t>
+  </si>
+  <si>
+    <t>La colonne "Raison d'utilisation" détaille la fonctionnalité et ne justifie pas le protocole
+Pourquoi séparer les 2 manières de démarrer une partie si le protocole est le même ?
+Mise à jour des meilleurs temps/historique des parties sans mentionner comment on les consulte
+Aucune présentation de la fonctionnalité principale du projet : Jouer durant une partie
+Aucune présentation du clavardage également</t>
+  </si>
+  <si>
+    <t>3 Vue des processus /6</t>
+  </si>
+  <si>
+    <t>3 Description des paquets /12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demander un indice : manque le nom de l'acteur (Player1 basé sur les autres diagrammes)
+Voir l'historique : manque les messages de retour pour afficher les historiques à l'utilisateur. La suppression doit être un [opt] et non une partie obligatoire de la séquence. Vous ne sauvegardez pas l'historique sur votre BD ?
+Connexion : entrerNom() doit être avant vérifierNom().  Acteur "Joueur 1" et non "Player 1" comme dans les autres diagrammes.
+Joueur une partie : bloquerUneSeconde() n'est que pour le joueur ayant fait l'erreur. Manque la notation [alt] ou [opt] pour différencier une erreur d'une différence trouvée : la séquence présentée assume que  Player 2 va toujours se tromper en premier et Player 1 va toujours trouver la différence.
+Jouer une partie : l'abandon d'un joueur permet à l'autre de continuer le jeu en mode solo. La séquence présentée suppose qu'on peut jouer qu'avec 2 joueurs et jamais solo : diagramme à revoir.
+Reprise vidéo : les actions de pause/reprendre et recommencer devraient utiliser la notation [alt] ou [opt]. Le changement de vitesse peut se faire durant le visionnement. 
+2 diagrammes avec "GameInterface", 3 avec "Client" : quelle est la différence ?
+Manque un diagramme pour la fonctionnalité de réinitialisation et meilleurs temps (CU-3.0,4.0 et 5.0 dans la Figure 3)
+</t>
+  </si>
+  <si>
+    <t>Aucune description des interfaces et leur contenu. Ex : GameConfigConst, Game, ChatMessage, etc
+Aucun code de retour en cas de problème (40X/50X) pour vos réponses HTTP
+verifyIfGameExists (Get) : manque le paramètre nom dans l'URI. Comment faites-vous la différence avec GET api/games/:id si c'est la même URI ?
+getBestTimes (Get) : manque un / avant :id dans l'URI
+modifyGameConstants (Patch) : manque le 2e paramètre dans l'URI
+modifyGameHistory (Patch) : le commentaire laisse entendre que c'est une supression et non une mise à jour
+deleteAllGame (Delete) : le mot "delete" dans l'URI n'est pas une bonne pratique pour une API REST
+GameStarted : est-ce que Players est 1 objet ou un tableau ?
+UpdateWaitingPlayerNameList : manque le nom du joueur dans le contenu
+Manque l'événement "CheckIfPlayerNameIsAvailable"
+LocalMessage : est-ce que "message" est de type textMessage ou ChatMessage ? Ce n'est pas clair</t>
+  </si>
+  <si>
+    <t>4 Vue logique /6</t>
+  </si>
+  <si>
+    <t>Page 14 : manque des liens entre les paquetages : évitez les paquetages "flottants". Les sous-paquetages ne sont pas présentés dans les tableaux. N'est pas clair si "Canvas" dans "Vue de jeu" est le même paquetage que dans "Vue de création de jeu"
+Page 17 : même commentaire que page 14. Beaucoup de duplication d'information avec les tableaux de la page 16. Ex : la classe HintService dans "Logique des indices"
+Aucun diagramme de classes. Impossible de voir comment les différentes classes intéragissent ensemble et leurs liens. Section à revoir.</t>
+  </si>
+  <si>
+    <t>5 Vue de déploiement /2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manque le système d'exploitation des différents noeuds
+EC2 n'est pas un envrionnement d'exécution : ça devrait être NodeJS
+Manque la représentaiton du logiciel du serveur dynamique
+GitLabPages n'est pas un environnement d'exécution
+Manque une spécification pour le serveur statique : manque les artefacts (HTML,CSS,JS, assets) hébergés par le serveur statique
+Angular n'est pas une interface
+MongoDB Atlas est un service d'hébergement pour des instances MongoDB : vos boîtes sont inversées
+</t>
+  </si>
+  <si>
+    <t>Forme /1</t>
+  </si>
+  <si>
+    <t>Attention à la notation UML dans les sections 3,4 et 5
+Notions de [alt] et [opt] à revoir pour les diagrammes de séquences
+Les diagrammes et figures des sections 3 et 4 ne sont pas numérotés. Pas de titres à la section 4.
+Page 13 : vous présentez des paquetages et non des "diagrammes de paquetage"</t>
+  </si>
+  <si>
+    <t>Section 3 :
+Le nom de la méthode dans la 1re colonne porte à confusion : gardez le verbe HTTP seulement
+La route devrait commencer par /api/xyz : votre déploiement n'est plus sur localhost
+Séparez la présentation des corps des requêtes et les réponses
+Regroupez vos routes HTTP par fonctionnalité. Ex : deleteGameById devrait être proche de deleteAllGame
+Regroupez vos événements WS par fonctionnalité : Ex : RemoveDiff du Client et du Serveur
+Une colonne description peut être pratique pour vos WS : plusieurs événements ont des noms qui n'aident pas à comprendre leur utilisation</t>
+  </si>
+  <si>
+    <t>FOND</t>
+  </si>
+  <si>
+    <t>FORME</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamel:
+Bien!
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -532,7 +739,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -570,7 +776,6 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -578,7 +783,6 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -586,7 +790,6 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -629,7 +832,43 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -637,23 +876,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -797,8 +1023,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="54">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -1465,6 +1715,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1475,7 +1794,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2109,6 +2428,51 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="27" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2264,6 +2628,9 @@
     </xf>
     <xf numFmtId="2" fontId="17" fillId="20" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2654,10 +3021,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FA667-0374-4556-B71F-558CE1E91347}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A3:G7"/>
+  <dimension ref="A3:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2670,7 +3037,7 @@
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="40"/>
       <c r="B3" s="126" t="s">
         <v>0</v>
@@ -2690,10 +3057,13 @@
       <c r="G3" s="129" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="107" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="108">
         <f>(Fonctionnalités!E15)</f>
@@ -2715,22 +3085,23 @@
         <f>D4*F4</f>
         <v>17.303999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="111"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="112" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="113">
         <f>(Fonctionnalités!E28)</f>
-        <v>0</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="C5" s="113">
         <f>'Assurance Qualité'!F59</f>
-        <v>0</v>
+        <v>0.86250000000000004</v>
       </c>
       <c r="D5" s="113">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0</v>
+        <v>0.92880000000000007</v>
       </c>
       <c r="E5" s="114"/>
       <c r="F5" s="115">
@@ -2738,12 +3109,16 @@
       </c>
       <c r="G5" s="116">
         <f t="shared" ref="G5:G7" si="1">D5*F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18.576000000000001</v>
+      </c>
+      <c r="H5" s="116">
+        <f>AVERAGE(Documents!B18,Documents!F18)*5</f>
+        <v>3.4125000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="118">
         <f>(Fonctionnalités!E43)</f>
@@ -2765,10 +3140,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="121">
+        <f>AVERAGE(Documents!C18,Documents!G18)*5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="122" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="122"/>
@@ -2783,6 +3162,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H7" s="125"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2794,8 +3174,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2814,36 +3194,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="251" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="251"/>
-      <c r="C2" s="251"/>
-      <c r="D2" s="251"/>
-      <c r="E2" s="251"/>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
-      <c r="K2" s="251"/>
+      <c r="A2" s="266" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="266"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="266"/>
+      <c r="H2" s="266"/>
+      <c r="I2" s="266"/>
+      <c r="J2" s="266"/>
+      <c r="K2" s="266"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="252" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="252"/>
-      <c r="C4" s="252"/>
-      <c r="D4" s="252"/>
-      <c r="E4" s="252"/>
-      <c r="F4" s="252"/>
-      <c r="G4" s="252"/>
-      <c r="H4" s="252"/>
-      <c r="I4" s="252"/>
-      <c r="J4" s="252"/>
-      <c r="K4" s="252"/>
+      <c r="A4" s="267" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="267"/>
+      <c r="C4" s="267"/>
+      <c r="D4" s="267"/>
+      <c r="E4" s="267"/>
+      <c r="F4" s="267"/>
+      <c r="G4" s="267"/>
+      <c r="H4" s="267"/>
+      <c r="I4" s="267"/>
+      <c r="J4" s="267"/>
+      <c r="K4" s="267"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
@@ -2863,62 +3243,62 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="244" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="256" t="s">
+      <c r="A6" s="259" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="246" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="247"/>
-      <c r="E6" s="247"/>
-      <c r="F6" s="248" t="s">
+      <c r="B6" s="271" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="261" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="249"/>
-      <c r="H6" s="250"/>
-      <c r="I6" s="253" t="s">
+      <c r="D6" s="262"/>
+      <c r="E6" s="262"/>
+      <c r="F6" s="263" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="254"/>
-      <c r="K6" s="255"/>
+      <c r="G6" s="264"/>
+      <c r="H6" s="265"/>
+      <c r="I6" s="268" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="269"/>
+      <c r="K6" s="270"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="242"/>
-      <c r="O6" s="243"/>
-      <c r="P6" s="243"/>
+      <c r="N6" s="257"/>
+      <c r="O6" s="258"/>
+      <c r="P6" s="258"/>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="245"/>
-      <c r="B7" s="257"/>
+      <c r="A7" s="260"/>
+      <c r="B7" s="272"/>
       <c r="C7" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>15</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>14</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>14</v>
       </c>
       <c r="J7" s="19" t="s">
         <v>4</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -2928,26 +3308,28 @@
       <c r="Q7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="226" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="226"/>
-      <c r="C8" s="219" t="s">
+      <c r="A8" s="241" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="220"/>
+      <c r="B8" s="241"/>
+      <c r="C8" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="235"/>
       <c r="E8" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="234" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="220"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="220"/>
+      <c r="G8" s="235"/>
+      <c r="H8" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="235"/>
       <c r="K8" s="46"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -2956,12 +3338,12 @@
       <c r="P8" s="40"/>
       <c r="Q8" s="40"/>
     </row>
-    <row r="9" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="100">
         <v>1</v>
@@ -2970,11 +3352,15 @@
         <v>6</v>
       </c>
       <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="F9" s="102">
+        <v>1</v>
+      </c>
       <c r="G9" s="99">
         <v>6</v>
       </c>
-      <c r="H9" s="103"/>
+      <c r="H9" s="103" t="s">
+        <v>22</v>
+      </c>
       <c r="I9" s="104"/>
       <c r="J9" s="105">
         <v>6</v>
@@ -2989,10 +3375,10 @@
     </row>
     <row r="10" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="100">
         <v>1</v>
@@ -3001,7 +3387,9 @@
         <v>2</v>
       </c>
       <c r="E10" s="101"/>
-      <c r="F10" s="102"/>
+      <c r="F10" s="102">
+        <v>1</v>
+      </c>
       <c r="G10" s="99">
         <v>2</v>
       </c>
@@ -3019,10 +3407,10 @@
       <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="1:17" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="221" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="222"/>
+      <c r="A11" s="236" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="237"/>
       <c r="C11" s="47">
         <f>SUMPRODUCT(C6:C10,D6:D10)</f>
         <v>8</v>
@@ -3034,7 +3422,7 @@
       <c r="E11" s="49"/>
       <c r="F11" s="50">
         <f>SUMPRODUCT(F6:F10,G6:G10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G11" s="51">
         <f>SUM(G6:G10)</f>
@@ -3058,26 +3446,28 @@
       <c r="Q11" s="44"/>
     </row>
     <row r="12" spans="1:17" s="12" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="226" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="226"/>
-      <c r="C12" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="220"/>
+      <c r="A12" s="241" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="241"/>
+      <c r="C12" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="235"/>
       <c r="E12" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="220"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="220"/>
+        <v>27</v>
+      </c>
+      <c r="F12" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="235"/>
+      <c r="H12" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="235"/>
       <c r="K12" s="46"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3086,12 +3476,12 @@
       <c r="P12" s="43"/>
       <c r="Q12" s="43"/>
     </row>
-    <row r="13" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="79">
         <v>0.75</v>
@@ -3100,14 +3490,18 @@
         <v>3</v>
       </c>
       <c r="E13" s="81" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="89"/>
+        <v>30</v>
+      </c>
+      <c r="F13" s="89">
+        <v>0.85</v>
+      </c>
       <c r="G13" s="90">
         <f>D13</f>
         <v>3</v>
       </c>
-      <c r="H13" s="91"/>
+      <c r="H13" s="91" t="s">
+        <v>31</v>
+      </c>
       <c r="I13" s="92"/>
       <c r="J13" s="93">
         <f>G13</f>
@@ -3117,12 +3511,12 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="272" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C14" s="83">
         <v>0.8</v>
@@ -3131,14 +3525,18 @@
         <v>2</v>
       </c>
       <c r="E14" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="86"/>
+        <v>34</v>
+      </c>
+      <c r="F14" s="86">
+        <v>0.45</v>
+      </c>
       <c r="G14" s="90">
         <f t="shared" ref="G14:G17" si="0">D14</f>
         <v>2</v>
       </c>
-      <c r="H14" s="88"/>
+      <c r="H14" s="88" t="s">
+        <v>35</v>
+      </c>
       <c r="I14" s="76"/>
       <c r="J14" s="93">
         <f t="shared" ref="J14:J17" si="1">G14</f>
@@ -3148,12 +3546,12 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="192" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C15" s="83">
         <v>0.55000000000000004</v>
@@ -3162,14 +3560,18 @@
         <v>2</v>
       </c>
       <c r="E15" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="86"/>
+        <v>38</v>
+      </c>
+      <c r="F15" s="86">
+        <v>0</v>
+      </c>
       <c r="G15" s="90">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H15" s="88"/>
+      <c r="H15" s="88" t="s">
+        <v>39</v>
+      </c>
       <c r="I15" s="76"/>
       <c r="J15" s="93">
         <f t="shared" si="1"/>
@@ -3181,10 +3583,10 @@
     </row>
     <row r="16" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C16" s="83">
         <v>1</v>
@@ -3193,7 +3595,9 @@
         <v>4</v>
       </c>
       <c r="E16" s="85"/>
-      <c r="F16" s="86"/>
+      <c r="F16" s="86">
+        <v>1</v>
+      </c>
       <c r="G16" s="90">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3210,10 +3614,10 @@
     </row>
     <row r="17" spans="1:17" ht="128" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C17" s="83">
         <v>0</v>
@@ -3222,14 +3626,18 @@
         <v>4</v>
       </c>
       <c r="E17" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="86"/>
+        <v>44</v>
+      </c>
+      <c r="F17" s="86">
+        <v>0.85</v>
+      </c>
       <c r="G17" s="90">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H17" s="88"/>
+      <c r="H17" s="88" t="s">
+        <v>45</v>
+      </c>
       <c r="I17" s="76"/>
       <c r="J17" s="93">
         <f t="shared" si="1"/>
@@ -3240,10 +3648,10 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="221" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="222"/>
+      <c r="A18" s="236" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="237"/>
       <c r="C18" s="47">
         <f>SUMPRODUCT(C13:C17,D13:D17)</f>
         <v>8.9499999999999993</v>
@@ -3255,7 +3663,7 @@
       <c r="E18" s="49"/>
       <c r="F18" s="50">
         <f>SUMPRODUCT(F13:F17,G13:G17)</f>
-        <v>0</v>
+        <v>10.85</v>
       </c>
       <c r="G18" s="51">
         <f>SUM(G13:G17)</f>
@@ -3279,36 +3687,38 @@
       <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17" s="43" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="258" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="258"/>
-      <c r="C19" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="220"/>
+      <c r="A19" s="273" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="273"/>
+      <c r="C19" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="235"/>
       <c r="E19" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="220"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="220"/>
+        <v>47</v>
+      </c>
+      <c r="F19" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="235"/>
+      <c r="H19" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="235"/>
       <c r="K19" s="46"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:17" ht="128" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="176" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C20" s="83">
         <v>0</v>
@@ -3317,13 +3727,17 @@
         <v>3</v>
       </c>
       <c r="E20" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="86"/>
+        <v>50</v>
+      </c>
+      <c r="F20" s="86">
+        <v>0.3</v>
+      </c>
       <c r="G20" s="87">
         <v>3</v>
       </c>
-      <c r="H20" s="88"/>
+      <c r="H20" s="88" t="s">
+        <v>51</v>
+      </c>
       <c r="I20" s="76"/>
       <c r="J20" s="77">
         <v>3</v>
@@ -3334,10 +3748,10 @@
     </row>
     <row r="21" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C21" s="83">
         <v>1</v>
@@ -3346,7 +3760,9 @@
         <v>3</v>
       </c>
       <c r="E21" s="85"/>
-      <c r="F21" s="86"/>
+      <c r="F21" s="86">
+        <v>1</v>
+      </c>
       <c r="G21" s="87">
         <v>3</v>
       </c>
@@ -3360,10 +3776,10 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="259" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="241"/>
+      <c r="A22" s="274" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="256"/>
       <c r="C22" s="57">
         <f>SUMPRODUCT(C20:C21,D20:D21)</f>
         <v>3</v>
@@ -3375,7 +3791,7 @@
       <c r="E22" s="59"/>
       <c r="F22" s="60">
         <f>SUMPRODUCT(F20:F21,G20:G21)</f>
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="G22" s="61">
         <f>SUM(G20:G21)</f>
@@ -3396,35 +3812,37 @@
     </row>
     <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="214" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B23" s="214"/>
-      <c r="C23" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="220"/>
+      <c r="C23" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="235"/>
       <c r="E23" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="234" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="220"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="220"/>
+      <c r="G23" s="235"/>
+      <c r="H23" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="235"/>
       <c r="K23" s="46"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="42" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C24" s="97">
         <v>1</v>
@@ -3433,7 +3851,9 @@
         <v>1</v>
       </c>
       <c r="E24" s="26"/>
-      <c r="F24" s="82"/>
+      <c r="F24" s="82">
+        <v>1</v>
+      </c>
       <c r="G24" s="27">
         <v>1</v>
       </c>
@@ -3448,10 +3868,10 @@
     </row>
     <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C25" s="83">
         <v>0.9</v>
@@ -3460,9 +3880,11 @@
         <v>2</v>
       </c>
       <c r="E25" s="85" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="86"/>
+        <v>59</v>
+      </c>
+      <c r="F25" s="86">
+        <v>1</v>
+      </c>
       <c r="G25" s="87">
         <v>2</v>
       </c>
@@ -3477,10 +3899,10 @@
     </row>
     <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C26" s="83">
         <v>1</v>
@@ -3489,7 +3911,9 @@
         <v>1</v>
       </c>
       <c r="E26" s="85"/>
-      <c r="F26" s="86"/>
+      <c r="F26" s="86">
+        <v>1</v>
+      </c>
       <c r="G26" s="87">
         <v>1</v>
       </c>
@@ -3503,10 +3927,10 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="240" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="241"/>
+      <c r="A27" s="255" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="256"/>
       <c r="C27" s="47">
         <f>SUMPRODUCT(C24:C26,D24:D26)</f>
         <v>3.8</v>
@@ -3518,7 +3942,7 @@
       <c r="E27" s="49"/>
       <c r="F27" s="60">
         <f>SUMPRODUCT(F24:F26,G24:G26)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G27" s="61">
         <f>SUM(G24:G26)</f>
@@ -3538,36 +3962,38 @@
       <c r="M27" s="56"/>
     </row>
     <row r="28" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="258" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="258"/>
-      <c r="C28" s="219">
-        <v>1</v>
-      </c>
-      <c r="D28" s="220"/>
+      <c r="A28" s="273" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="273"/>
+      <c r="C28" s="234">
+        <v>1</v>
+      </c>
+      <c r="D28" s="235"/>
       <c r="E28" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="220"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="220"/>
+        <v>47</v>
+      </c>
+      <c r="F28" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="235"/>
+      <c r="H28" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="235"/>
       <c r="K28" s="46"/>
       <c r="L28" s="9"/>
       <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C29" s="79">
         <v>0.7</v>
@@ -3576,14 +4002,18 @@
         <v>2</v>
       </c>
       <c r="E29" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="89"/>
+        <v>65</v>
+      </c>
+      <c r="F29" s="89">
+        <v>1</v>
+      </c>
       <c r="G29" s="90">
         <f>D29</f>
         <v>2</v>
       </c>
-      <c r="H29" s="95"/>
+      <c r="H29" s="95" t="s">
+        <v>66</v>
+      </c>
       <c r="I29" s="92"/>
       <c r="J29" s="93">
         <f>D29</f>
@@ -3595,10 +4025,10 @@
     </row>
     <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C30" s="83">
         <v>1</v>
@@ -3607,7 +4037,9 @@
         <v>2</v>
       </c>
       <c r="E30" s="85"/>
-      <c r="F30" s="86"/>
+      <c r="F30" s="86">
+        <v>1</v>
+      </c>
       <c r="G30" s="90">
         <f t="shared" ref="G30:G31" si="2">D30</f>
         <v>2</v>
@@ -3622,12 +4054,12 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C31" s="83">
         <v>1</v>
@@ -3636,12 +4068,16 @@
         <v>2</v>
       </c>
       <c r="E31" s="85"/>
-      <c r="F31" s="86"/>
+      <c r="F31" s="86">
+        <v>0.8</v>
+      </c>
       <c r="G31" s="90">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H31" s="96"/>
+      <c r="H31" s="96" t="s">
+        <v>71</v>
+      </c>
       <c r="I31" s="76"/>
       <c r="J31" s="93">
         <f t="shared" si="3"/>
@@ -3652,10 +4088,10 @@
       <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="221" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="222"/>
+      <c r="A32" s="236" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="237"/>
       <c r="C32" s="47">
         <f>SUMPRODUCT(C29:C31,D29:D31)</f>
         <v>5.4</v>
@@ -3667,7 +4103,7 @@
       <c r="E32" s="49"/>
       <c r="F32" s="50">
         <f>SUMPRODUCT(F29:F31,G29:G31)</f>
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G32" s="51">
         <f>SUM(G29:G31)</f>
@@ -3687,36 +4123,38 @@
       <c r="M32" s="56"/>
     </row>
     <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="226" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="226"/>
-      <c r="C33" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="220"/>
+      <c r="A33" s="241" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="241"/>
+      <c r="C33" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="235"/>
       <c r="E33" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="220"/>
-      <c r="H33" s="46"/>
+        <v>27</v>
+      </c>
+      <c r="F33" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="235"/>
+      <c r="H33" s="46" t="s">
+        <v>27</v>
+      </c>
       <c r="I33" s="68" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J33" s="66"/>
       <c r="K33" s="46"/>
       <c r="L33" s="8"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C34" s="79">
         <v>1</v>
@@ -3725,11 +4163,15 @@
         <v>2</v>
       </c>
       <c r="E34" s="81"/>
-      <c r="F34" s="89"/>
+      <c r="F34" s="89">
+        <v>0.9</v>
+      </c>
       <c r="G34" s="90">
         <v>2</v>
       </c>
-      <c r="H34" s="91"/>
+      <c r="H34" s="91" t="s">
+        <v>75</v>
+      </c>
       <c r="I34" s="92"/>
       <c r="J34" s="93">
         <v>2</v>
@@ -3740,10 +4182,10 @@
     </row>
     <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C35" s="83">
         <v>1</v>
@@ -3752,7 +4194,9 @@
         <v>2</v>
       </c>
       <c r="E35" s="85"/>
-      <c r="F35" s="86"/>
+      <c r="F35" s="86">
+        <v>1</v>
+      </c>
       <c r="G35" s="87">
         <v>2</v>
       </c>
@@ -3765,12 +4209,12 @@
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C36" s="83">
         <v>0.85</v>
@@ -3779,13 +4223,17 @@
         <v>3</v>
       </c>
       <c r="E36" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="86"/>
+        <v>80</v>
+      </c>
+      <c r="F36" s="86">
+        <v>0.85</v>
+      </c>
       <c r="G36" s="87">
         <v>3</v>
       </c>
-      <c r="H36" s="88"/>
+      <c r="H36" s="88" t="s">
+        <v>81</v>
+      </c>
       <c r="I36" s="76"/>
       <c r="J36" s="77">
         <v>3</v>
@@ -3796,10 +4244,10 @@
     </row>
     <row r="37" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C37" s="83">
         <v>1</v>
@@ -3808,11 +4256,15 @@
         <v>3</v>
       </c>
       <c r="E37" s="85"/>
-      <c r="F37" s="86"/>
+      <c r="F37" s="86">
+        <v>0.85</v>
+      </c>
       <c r="G37" s="87">
         <v>3</v>
       </c>
-      <c r="H37" s="88"/>
+      <c r="H37" s="88" t="s">
+        <v>84</v>
+      </c>
       <c r="I37" s="76"/>
       <c r="J37" s="77">
         <v>3</v>
@@ -3821,11 +4273,11 @@
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="221" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="222"/>
+    <row r="38" spans="1:13" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="236" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="237"/>
       <c r="C38" s="69">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
         <v>9.5500000000000007</v>
@@ -3837,13 +4289,15 @@
       <c r="E38" s="49"/>
       <c r="F38" s="70">
         <f>SUMPRODUCT(F34:F37,G34:G37)</f>
-        <v>0</v>
+        <v>8.8999999999999986</v>
       </c>
       <c r="G38" s="51">
         <f>SUM(G34:G37)</f>
         <v>10</v>
       </c>
-      <c r="H38" s="52"/>
+      <c r="H38" s="52" t="s">
+        <v>85</v>
+      </c>
       <c r="I38" s="63">
         <f>SUMPRODUCT(I34:I37,J34:J37)</f>
         <v>0</v>
@@ -3858,35 +4312,35 @@
     </row>
     <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="45" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B39" s="45"/>
-      <c r="C39" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="220"/>
+      <c r="C39" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="235"/>
       <c r="E39" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="220"/>
+        <v>87</v>
+      </c>
+      <c r="F39" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="235"/>
       <c r="H39" s="46"/>
-      <c r="I39" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="220"/>
+      <c r="I39" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="235"/>
       <c r="K39" s="46"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C40" s="83">
         <v>1</v>
@@ -3895,14 +4349,18 @@
         <v>2</v>
       </c>
       <c r="E40" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="86"/>
+        <v>27</v>
+      </c>
+      <c r="F40" s="86">
+        <v>1</v>
+      </c>
       <c r="G40" s="87">
         <f>D40</f>
         <v>2</v>
       </c>
-      <c r="H40" s="88"/>
+      <c r="H40" s="88" t="s">
+        <v>27</v>
+      </c>
       <c r="I40" s="76"/>
       <c r="J40" s="77">
         <f>D40</f>
@@ -3914,10 +4372,10 @@
     </row>
     <row r="41" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C41" s="83">
         <v>0.7</v>
@@ -3926,14 +4384,18 @@
         <v>2</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>79</v>
-      </c>
-      <c r="F41" s="86"/>
+        <v>92</v>
+      </c>
+      <c r="F41" s="86">
+        <v>1</v>
+      </c>
       <c r="G41" s="87">
         <f t="shared" ref="G41:G48" si="4">D41</f>
         <v>2</v>
       </c>
-      <c r="H41" s="88"/>
+      <c r="H41" s="88" t="s">
+        <v>19</v>
+      </c>
       <c r="I41" s="76"/>
       <c r="J41" s="77">
         <f t="shared" ref="J41:J48" si="5">D41</f>
@@ -3943,12 +4405,12 @@
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C42" s="83">
         <v>1</v>
@@ -3957,14 +4419,18 @@
         <v>2</v>
       </c>
       <c r="E42" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="86"/>
+        <v>19</v>
+      </c>
+      <c r="F42" s="86">
+        <v>1</v>
+      </c>
       <c r="G42" s="87">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H42" s="88"/>
+      <c r="H42" s="88" t="s">
+        <v>95</v>
+      </c>
       <c r="I42" s="76"/>
       <c r="J42" s="77">
         <f t="shared" si="5"/>
@@ -3975,10 +4441,10 @@
     </row>
     <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C43" s="83">
         <v>0.8</v>
@@ -3987,14 +4453,18 @@
         <v>4</v>
       </c>
       <c r="E43" s="85" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" s="86"/>
+        <v>98</v>
+      </c>
+      <c r="F43" s="86">
+        <v>1</v>
+      </c>
       <c r="G43" s="87">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="H43" s="88"/>
+      <c r="H43" s="88" t="s">
+        <v>19</v>
+      </c>
       <c r="I43" s="76"/>
       <c r="J43" s="77">
         <f t="shared" si="5"/>
@@ -4004,12 +4474,12 @@
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
     </row>
-    <row r="44" spans="1:13" ht="128" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="304" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C44" s="83">
         <v>0</v>
@@ -4018,14 +4488,18 @@
         <v>6</v>
       </c>
       <c r="E44" s="85" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="86"/>
+        <v>101</v>
+      </c>
+      <c r="F44" s="86">
+        <v>0.4</v>
+      </c>
       <c r="G44" s="87">
-        <f t="shared" si="4"/>
+        <f>D44</f>
         <v>6</v>
       </c>
-      <c r="H44" s="88"/>
+      <c r="H44" s="88" t="s">
+        <v>102</v>
+      </c>
       <c r="I44" s="76"/>
       <c r="J44" s="77">
         <f t="shared" si="5"/>
@@ -4037,10 +4511,10 @@
     </row>
     <row r="45" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C45" s="83">
         <v>1</v>
@@ -4049,14 +4523,18 @@
         <v>8</v>
       </c>
       <c r="E45" s="85" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="86"/>
+        <v>47</v>
+      </c>
+      <c r="F45" s="86">
+        <v>1</v>
+      </c>
       <c r="G45" s="87">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H45" s="88"/>
+      <c r="H45" s="88" t="s">
+        <v>190</v>
+      </c>
       <c r="I45" s="76"/>
       <c r="J45" s="77">
         <f t="shared" si="5"/>
@@ -4068,10 +4546,10 @@
     </row>
     <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C46" s="83">
         <v>1</v>
@@ -4080,14 +4558,18 @@
         <v>6</v>
       </c>
       <c r="E46" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="86"/>
+        <v>27</v>
+      </c>
+      <c r="F46" s="86">
+        <v>1</v>
+      </c>
       <c r="G46" s="87">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="H46" s="88"/>
+      <c r="H46" s="88" t="s">
+        <v>27</v>
+      </c>
       <c r="I46" s="76"/>
       <c r="J46" s="77">
         <f t="shared" si="5"/>
@@ -4097,12 +4579,12 @@
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
     </row>
-    <row r="47" spans="1:13" ht="192" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="224" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C47" s="83">
         <v>0.3</v>
@@ -4111,14 +4593,18 @@
         <v>6</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="F47" s="86"/>
+        <v>109</v>
+      </c>
+      <c r="F47" s="86">
+        <v>0.6</v>
+      </c>
       <c r="G47" s="87">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="H47" s="88"/>
+      <c r="H47" s="88" t="s">
+        <v>110</v>
+      </c>
       <c r="I47" s="76"/>
       <c r="J47" s="77">
         <f t="shared" si="5"/>
@@ -4130,10 +4616,10 @@
     </row>
     <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C48" s="83">
         <v>1</v>
@@ -4142,14 +4628,18 @@
         <v>4</v>
       </c>
       <c r="E48" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="86"/>
+        <v>19</v>
+      </c>
+      <c r="F48" s="86">
+        <v>1</v>
+      </c>
       <c r="G48" s="87">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="H48" s="88"/>
+      <c r="H48" s="88" t="s">
+        <v>19</v>
+      </c>
       <c r="I48" s="76"/>
       <c r="J48" s="77">
         <f t="shared" si="5"/>
@@ -4160,10 +4650,10 @@
       <c r="M48" s="5"/>
     </row>
     <row r="49" spans="1:17" s="30" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="221" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="222"/>
+      <c r="A49" s="236" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="237"/>
       <c r="C49" s="71">
         <f>SUMPRODUCT(C40:C48,D40:D48)</f>
         <v>28.400000000000002</v>
@@ -4175,7 +4665,7 @@
       <c r="E49" s="59"/>
       <c r="F49" s="70">
         <f>SUMPRODUCT(F40:F48,G40:G48)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G49" s="51">
         <f>SUM(G40:G48)</f>
@@ -4199,36 +4689,38 @@
       <c r="Q49" s="44"/>
     </row>
     <row r="50" spans="1:17" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="226" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="226"/>
-      <c r="C50" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="220"/>
+      <c r="A50" s="241" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="241"/>
+      <c r="C50" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="235"/>
       <c r="E50" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="G50" s="220"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="219" t="s">
-        <v>17</v>
-      </c>
-      <c r="J50" s="220"/>
+        <v>47</v>
+      </c>
+      <c r="F50" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="235"/>
+      <c r="H50" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="I50" s="234" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="235"/>
       <c r="K50" s="46"/>
       <c r="L50" s="8"/>
       <c r="M50" s="4"/>
     </row>
     <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="29" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C51" s="79">
         <v>1</v>
@@ -4237,7 +4729,9 @@
         <v>2</v>
       </c>
       <c r="E51" s="81"/>
-      <c r="F51" s="82"/>
+      <c r="F51" s="82">
+        <v>1</v>
+      </c>
       <c r="G51" s="27">
         <v>2</v>
       </c>
@@ -4252,10 +4746,10 @@
     </row>
     <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C52" s="83">
         <v>1</v>
@@ -4264,7 +4758,9 @@
         <v>2</v>
       </c>
       <c r="E52" s="85"/>
-      <c r="F52" s="86"/>
+      <c r="F52" s="86">
+        <v>1</v>
+      </c>
       <c r="G52" s="87">
         <v>2</v>
       </c>
@@ -4279,10 +4775,10 @@
     </row>
     <row r="53" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="23" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C53" s="83">
         <v>1</v>
@@ -4291,7 +4787,9 @@
         <v>1</v>
       </c>
       <c r="E53" s="85"/>
-      <c r="F53" s="86"/>
+      <c r="F53" s="86">
+        <v>1</v>
+      </c>
       <c r="G53" s="87">
         <v>1</v>
       </c>
@@ -4306,10 +4804,10 @@
     </row>
     <row r="54" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C54" s="83">
         <v>1</v>
@@ -4318,7 +4816,9 @@
         <v>4</v>
       </c>
       <c r="E54" s="85"/>
-      <c r="F54" s="86"/>
+      <c r="F54" s="86">
+        <v>1</v>
+      </c>
       <c r="G54" s="87">
         <v>4</v>
       </c>
@@ -4333,10 +4833,10 @@
     </row>
     <row r="55" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="C55" s="83">
         <v>0.5</v>
@@ -4345,9 +4845,11 @@
         <v>2</v>
       </c>
       <c r="E55" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="F55" s="86"/>
+        <v>124</v>
+      </c>
+      <c r="F55" s="86">
+        <v>1</v>
+      </c>
       <c r="G55" s="87">
         <v>2</v>
       </c>
@@ -4360,11 +4862,11 @@
       <c r="L55" s="6"/>
       <c r="M55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="221" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" s="222"/>
+    <row r="56" spans="1:17" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="236" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="237"/>
       <c r="C56" s="57">
         <f>SUMPRODUCT(C51:C55,D51:D55)</f>
         <v>10</v>
@@ -4376,13 +4878,15 @@
       <c r="E56" s="59"/>
       <c r="F56" s="60">
         <f>SUMPRODUCT(F51:F55,G51:G55)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G56" s="61">
         <f>SUM(G51:G55)</f>
         <v>11</v>
       </c>
-      <c r="H56" s="62"/>
+      <c r="H56" s="62" t="s">
+        <v>125</v>
+      </c>
       <c r="I56" s="53">
         <f>SUMPRODUCT(I51:I55,J51:J55)</f>
         <v>0</v>
@@ -4396,27 +4900,27 @@
       <c r="M56" s="56"/>
     </row>
     <row r="57" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="223" t="s">
+      <c r="A57" s="238" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="224"/>
-      <c r="C57" s="224"/>
-      <c r="D57" s="224"/>
-      <c r="E57" s="224"/>
-      <c r="F57" s="224"/>
-      <c r="G57" s="224"/>
-      <c r="H57" s="224"/>
-      <c r="I57" s="224"/>
-      <c r="J57" s="224"/>
-      <c r="K57" s="225"/>
+      <c r="B57" s="239"/>
+      <c r="C57" s="239"/>
+      <c r="D57" s="239"/>
+      <c r="E57" s="239"/>
+      <c r="F57" s="239"/>
+      <c r="G57" s="239"/>
+      <c r="H57" s="239"/>
+      <c r="I57" s="239"/>
+      <c r="J57" s="239"/>
+      <c r="K57" s="240"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" s="227" t="s">
-        <v>109</v>
-      </c>
-      <c r="B58" s="228"/>
+      <c r="A58" s="242" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="243"/>
       <c r="C58" s="34">
         <f>C11+C18+C22+C27+C32+C38+C49+C56</f>
         <v>77.100000000000009</v>
@@ -4428,7 +4932,7 @@
       <c r="E58" s="26"/>
       <c r="F58" s="35">
         <f>F11+F18+F22+F27+F32+F38+F49+F56</f>
-        <v>0</v>
+        <v>86.25</v>
       </c>
       <c r="G58" s="27">
         <f>G11+G18+G22+G27+G32+G38+G49+G56</f>
@@ -4448,28 +4952,28 @@
       <c r="M58" s="5"/>
     </row>
     <row r="59" spans="1:17" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="229" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" s="230"/>
-      <c r="C59" s="231">
+      <c r="A59" s="244" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="245"/>
+      <c r="C59" s="246">
         <f>C58/D58</f>
         <v>0.77100000000000013</v>
       </c>
-      <c r="D59" s="232"/>
-      <c r="E59" s="233"/>
-      <c r="F59" s="234">
+      <c r="D59" s="247"/>
+      <c r="E59" s="248"/>
+      <c r="F59" s="249">
         <f>F58/G58</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="235"/>
-      <c r="H59" s="236"/>
-      <c r="I59" s="237">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="G59" s="250"/>
+      <c r="H59" s="251"/>
+      <c r="I59" s="252">
         <f>I58/J58</f>
         <v>0</v>
       </c>
-      <c r="J59" s="238"/>
-      <c r="K59" s="239"/>
+      <c r="J59" s="253"/>
+      <c r="K59" s="254"/>
       <c r="L59" s="72"/>
       <c r="M59" s="72"/>
     </row>
@@ -4547,8 +5051,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4563,15 +5067,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="260" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
+      <c r="A2" s="275" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="275"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
+      <c r="G2" s="275"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="38"/>
@@ -4584,7 +5088,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -4595,42 +5099,42 @@
     </row>
     <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="264" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="265"/>
-      <c r="C6" s="265"/>
-      <c r="D6" s="265"/>
-      <c r="E6" s="265"/>
-      <c r="F6" s="265"/>
-      <c r="G6" s="266"/>
+      <c r="A6" s="279" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="280"/>
+      <c r="C6" s="280"/>
+      <c r="D6" s="280"/>
+      <c r="E6" s="280"/>
+      <c r="F6" s="280"/>
+      <c r="G6" s="281"/>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="130" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B7" s="131" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="131" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D7" s="131" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F7" s="131" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="132" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="133" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B8" s="134">
         <v>1</v>
@@ -4646,13 +5150,13 @@
         <v>4</v>
       </c>
       <c r="F8" s="134" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G8" s="135"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="136" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B9" s="137">
         <v>1</v>
@@ -4668,13 +5172,13 @@
         <v>12</v>
       </c>
       <c r="F9" s="137" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G9" s="138"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B10" s="134">
         <v>1</v>
@@ -4690,13 +5194,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="134" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G10" s="135"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="136" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="B11" s="137">
         <v>0.8</v>
@@ -4712,15 +5216,15 @@
         <v>12.8</v>
       </c>
       <c r="F11" s="137" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="138" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="133" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B12" s="134">
         <v>0.8</v>
@@ -4736,15 +5240,15 @@
         <v>16</v>
       </c>
       <c r="F12" s="218" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="135" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="133" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B13" s="134">
         <v>1</v>
@@ -4760,13 +5264,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="134" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" s="135"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="136" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="B14" s="137">
         <v>1</v>
@@ -4782,16 +5286,16 @@
         <v>26</v>
       </c>
       <c r="F14" s="137" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="138"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="139" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="267"/>
-      <c r="C15" s="267"/>
+        <v>141</v>
+      </c>
+      <c r="B15" s="282"/>
+      <c r="C15" s="282"/>
       <c r="D15" s="140">
         <f>SUM(D8:D14)</f>
         <v>100</v>
@@ -4805,26 +5309,26 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="143" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B16" s="144" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="144"/>
       <c r="D16" s="144" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="145" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F16" s="145"/>
       <c r="G16" s="146" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="147" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B17" s="148"/>
       <c r="C17" s="148"/>
@@ -4836,13 +5340,13 @@
         <v>0</v>
       </c>
       <c r="F17" s="148" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" s="150"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="151" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B18" s="152">
         <v>0</v>
@@ -4859,182 +5363,200 @@
       <c r="G18" s="154"/>
     </row>
     <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="268" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="269"/>
-      <c r="C19" s="269"/>
-      <c r="D19" s="269"/>
-      <c r="E19" s="269"/>
-      <c r="F19" s="269"/>
-      <c r="G19" s="270"/>
+      <c r="A19" s="283" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="284"/>
+      <c r="C19" s="284"/>
+      <c r="D19" s="284"/>
+      <c r="E19" s="284"/>
+      <c r="F19" s="284"/>
+      <c r="G19" s="285"/>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="155" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B20" s="156" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" s="156" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D20" s="156" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="156" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F20" s="156" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G20" s="157" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="158" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B21" s="159">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C21" s="159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="159">
         <v>26</v>
       </c>
       <c r="E21" s="159">
         <f>B21*C21*D21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="159"/>
-      <c r="G21" s="160"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>24.7</v>
+      </c>
+      <c r="F21" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="160" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="161" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B22" s="162">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C22" s="162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="162">
         <v>14</v>
       </c>
       <c r="E22" s="162">
         <f t="shared" ref="E22:E27" si="1">B22*C22*D22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="162"/>
-      <c r="G22" s="163"/>
+        <v>12.6</v>
+      </c>
+      <c r="F22" s="162" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="219" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="158" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="B23" s="159">
-        <v>0</v>
-      </c>
-      <c r="C23" s="159">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C23" s="162">
+        <v>1</v>
       </c>
       <c r="D23" s="159">
         <v>26</v>
       </c>
       <c r="E23" s="159">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="159"/>
+        <v>26</v>
+      </c>
+      <c r="F23" s="159" t="s">
+        <v>19</v>
+      </c>
       <c r="G23" s="160"/>
     </row>
     <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="161" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B24" s="162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="162">
         <v>12</v>
       </c>
       <c r="E24" s="162">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="162"/>
+        <v>12</v>
+      </c>
+      <c r="F24" s="162" t="s">
+        <v>19</v>
+      </c>
       <c r="G24" s="163"/>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="158" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="B25" s="159">
-        <v>0</v>
-      </c>
-      <c r="C25" s="159">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="162">
+        <v>1</v>
       </c>
       <c r="D25" s="159">
         <v>8</v>
       </c>
       <c r="E25" s="159">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="159"/>
+        <v>8</v>
+      </c>
+      <c r="F25" s="159" t="s">
+        <v>19</v>
+      </c>
       <c r="G25" s="160"/>
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="161" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="B26" s="162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="162">
         <v>6</v>
       </c>
       <c r="E26" s="162">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="162"/>
+        <f>B26*C26*D26</f>
+        <v>6</v>
+      </c>
+      <c r="F26" s="162" t="s">
+        <v>19</v>
+      </c>
       <c r="G26" s="163"/>
     </row>
     <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="215" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B27" s="215">
-        <v>0</v>
-      </c>
-      <c r="C27" s="215">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="162">
+        <v>1</v>
       </c>
       <c r="D27" s="215">
         <v>8</v>
       </c>
       <c r="E27" s="162">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="215"/>
+        <v>8</v>
+      </c>
+      <c r="F27" s="162" t="s">
+        <v>19</v>
+      </c>
       <c r="G27" s="216"/>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="164" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B28" s="165"/>
       <c r="C28" s="165"/>
@@ -5043,34 +5565,34 @@
         <v>100</v>
       </c>
       <c r="E28" s="166">
-        <f>(SUM(E21:E26) + E30+E31+E32)/D28</f>
-        <v>0</v>
+        <f>(SUM(E21:E27) + E30+E31+E32)/D28</f>
+        <v>0.97299999999999998</v>
       </c>
       <c r="F28" s="166"/>
       <c r="G28" s="167"/>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="168" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B29" s="169" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" s="169"/>
       <c r="D29" s="169" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="170" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F29" s="170"/>
       <c r="G29" s="171" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="172" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B30" s="173">
         <v>0</v>
@@ -5088,7 +5610,7 @@
     </row>
     <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="176" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="B31" s="177">
         <v>0</v>
@@ -5106,7 +5628,7 @@
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="180" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B32" s="181">
         <v>0</v>
@@ -5123,42 +5645,42 @@
       <c r="G32" s="183"/>
     </row>
     <row r="33" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A33" s="261" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="262"/>
-      <c r="C33" s="262"/>
-      <c r="D33" s="262"/>
-      <c r="E33" s="262"/>
-      <c r="F33" s="262"/>
-      <c r="G33" s="263"/>
+      <c r="A33" s="276" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="277"/>
+      <c r="C33" s="277"/>
+      <c r="D33" s="277"/>
+      <c r="E33" s="277"/>
+      <c r="F33" s="277"/>
+      <c r="G33" s="278"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="184" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B34" s="185" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" s="185" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D34" s="185" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="185" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F34" s="185" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G34" s="186" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="187" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="B35" s="188">
         <v>0</v>
@@ -5178,7 +5700,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="190" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="B36" s="191">
         <v>0</v>
@@ -5198,7 +5720,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="187" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B37" s="188">
         <v>0</v>
@@ -5218,7 +5740,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="190" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B38" s="191">
         <v>0</v>
@@ -5238,7 +5760,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="187" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B39" s="188">
         <v>0</v>
@@ -5258,7 +5780,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="190" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="B40" s="191">
         <v>0</v>
@@ -5278,7 +5800,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="187" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B41" s="188">
         <v>0</v>
@@ -5298,7 +5820,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="217" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B42" s="217">
         <v>0</v>
@@ -5318,7 +5840,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="193" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B43" s="194"/>
       <c r="C43" s="194"/>
@@ -5327,7 +5849,7 @@
         <v>100</v>
       </c>
       <c r="E43" s="195">
-        <f>(SUM(E35:E41) +E45+E46+E47)/D43</f>
+        <f>(SUM(E35:E42) +E45+E46+E47)/D43</f>
         <v>0</v>
       </c>
       <c r="F43" s="195"/>
@@ -5335,26 +5857,26 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="197" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B44" s="198" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C44" s="198"/>
       <c r="D44" s="198" t="s">
         <v>4</v>
       </c>
       <c r="E44" s="199" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F44" s="199"/>
       <c r="G44" s="200" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="201" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B45" s="202">
         <v>0</v>
@@ -5372,7 +5894,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="205" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="B46" s="206">
         <v>0</v>
@@ -5390,7 +5912,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="209" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B47" s="210">
         <v>0</v>
@@ -5429,6 +5951,277 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101BADF3-C115-4BB7-A238-E0CBC556CE80}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="88.83203125" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="286" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="286"/>
+      <c r="E1" s="286" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="286"/>
+    </row>
+    <row r="2" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="233" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="233" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="233" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="220" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="226" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="220" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="226"/>
+    </row>
+    <row r="4" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="221" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="227">
+        <v>1</v>
+      </c>
+      <c r="C4" s="227"/>
+      <c r="E4" s="221" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="227">
+        <v>1</v>
+      </c>
+      <c r="G4" s="227"/>
+    </row>
+    <row r="5" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="220"/>
+      <c r="B5" s="228" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="220" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="228" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="221" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="227">
+        <v>4</v>
+      </c>
+      <c r="C6" s="227"/>
+      <c r="E6" s="221" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="227">
+        <v>4</v>
+      </c>
+      <c r="G6" s="227"/>
+    </row>
+    <row r="7" spans="1:7" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="220"/>
+      <c r="B7" s="226" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="220"/>
+      <c r="F7" s="226" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="221" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="227">
+        <v>4.5</v>
+      </c>
+      <c r="C8" s="227"/>
+      <c r="E8" s="221" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="227">
+        <v>8</v>
+      </c>
+      <c r="G8" s="227"/>
+    </row>
+    <row r="9" spans="1:7" ht="359.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="220"/>
+      <c r="B9" s="229" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" s="222"/>
+      <c r="F9" s="229" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="221" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="227">
+        <v>3.5</v>
+      </c>
+      <c r="C10" s="227"/>
+    </row>
+    <row r="11" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="220"/>
+      <c r="B11" s="229" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="221" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="227">
+        <v>1</v>
+      </c>
+      <c r="C12" s="227"/>
+    </row>
+    <row r="13" spans="1:7" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="222"/>
+      <c r="B13" s="229" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="223" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="227">
+        <v>0.75</v>
+      </c>
+      <c r="C14" s="227"/>
+      <c r="E14" s="223" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="232">
+        <v>0.75</v>
+      </c>
+      <c r="G14" s="227"/>
+    </row>
+    <row r="15" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="A15" s="220"/>
+      <c r="B15" s="229" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="220"/>
+      <c r="F15" s="229" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="224" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="230">
+        <f>SUM(B4,B6,B8,B10,B12)</f>
+        <v>14</v>
+      </c>
+      <c r="C16" s="230">
+        <f>SUM(C4,C6,C8,C10,C12)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="224" t="s">
+        <v>187</v>
+      </c>
+      <c r="F16" s="230">
+        <f>SUM(F4,F6,F8)</f>
+        <v>13</v>
+      </c>
+      <c r="G16" s="230">
+        <f>SUM(G4,G6,G8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="224" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="230">
+        <f>B14</f>
+        <v>0.75</v>
+      </c>
+      <c r="C17" s="230">
+        <f>C14</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="224" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="230">
+        <f>F14</f>
+        <v>0.75</v>
+      </c>
+      <c r="G17" s="230">
+        <f>G14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="225" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="231">
+        <f>B16/20*0.9+B17*0.1</f>
+        <v>0.70500000000000007</v>
+      </c>
+      <c r="C18" s="231">
+        <f>C16/20*0.9+C17*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="225" t="s">
+        <v>189</v>
+      </c>
+      <c r="F18" s="231">
+        <f>F16/20*0.9+F17*0.1</f>
+        <v>0.66000000000000014</v>
+      </c>
+      <c r="G18" s="231">
+        <f>G16/20*0.9+G17*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>